<commit_message>
updated literature and documentation
</commit_message>
<xml_diff>
--- a/doc/Project_Structure.xlsx
+++ b/doc/Project_Structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Master\Master Biologie\Sommersemester 2022\Master thesis\ml_coda\ml_benchmarking_R\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Master\Master Biologie\Sommersemester 2022\Master thesis\Github\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CFA7A1-76EC-460F-A4E2-2B4D82B28B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D901FA6-E069-4A8C-90AC-AB13A0DD2AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="103">
   <si>
     <t>Projektstrukturplan</t>
   </si>
@@ -120,12 +120,6 @@
   </si>
   <si>
     <t>31.07.22</t>
-  </si>
-  <si>
-    <t>Work Block 2</t>
-  </si>
-  <si>
-    <t>Work Block 3</t>
   </si>
   <si>
     <t>Presentation/Defense Master Thesis</t>
@@ -332,6 +326,30 @@
   </si>
   <si>
     <t>22.02.2022</t>
+  </si>
+  <si>
+    <t>Establishing Data</t>
+  </si>
+  <si>
+    <t>Summarizing Data</t>
+  </si>
+  <si>
+    <t>31.03.: rejected; good pipeline exists with mikropml</t>
+  </si>
+  <si>
+    <t>31.03.22</t>
+  </si>
+  <si>
+    <t>31.04.22</t>
+  </si>
+  <si>
+    <t>31.03.: almost done, access to HPC required for transformations for EstMB</t>
+  </si>
+  <si>
+    <t>15.05.22</t>
+  </si>
+  <si>
+    <t>07.06.22</t>
   </si>
 </sst>
 </file>
@@ -726,16 +744,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>119884</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>119883</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>94544</xdr:rowOff>
+      <xdr:rowOff>58685</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>122814</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>122813</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>100405</xdr:rowOff>
+      <xdr:rowOff>64546</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -750,8 +768,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7838496" y="865509"/>
-          <a:ext cx="2930" cy="4129625"/>
+          <a:off x="8932189" y="829650"/>
+          <a:ext cx="2930" cy="4506143"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -782,76 +800,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>95475</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>148706</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>131334</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>166635</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>107577</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="Isosceles Triangle 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{896F49CE-6379-4DCC-95DA-F49F7F6CC624}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11695804" y="4326259"/>
-          <a:ext cx="236220" cy="182988"/>
-        </a:xfrm>
-        <a:prstGeom prst="triangle">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent6">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1800"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>104439</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>139741</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>116542</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>143436</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>143435</xdr:rowOff>
+      <xdr:rowOff>170329</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -866,7 +824,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12153004" y="4496588"/>
+          <a:off x="11435828" y="4344188"/>
           <a:ext cx="236220" cy="182988"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -964,21 +922,21 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>59615</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>148706</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>175600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>71717</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Isosceles Triangle 17">
+        <xdr:cNvPr id="7" name="Isosceles Triangle 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{367D8B1C-4B92-4920-B79E-A2977F90304F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C7E0C3A-02BF-4632-8495-DB64A420F573}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -986,8 +944,68 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10691756" y="3788377"/>
+          <a:off x="10691756" y="3994565"/>
           <a:ext cx="236220" cy="182988"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>77544</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>354894</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>89645</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>170330</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Isosceles Triangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80F0666C-B621-4452-A60B-EC07DF386375}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10682791" y="4182823"/>
+          <a:ext cx="236219" cy="182989"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst/>
@@ -1338,14 +1356,14 @@
   <dimension ref="A1:AF26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B6" sqref="B6:AF26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="37.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" customWidth="1"/>
     <col min="5" max="32" width="3.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1359,7 +1377,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
@@ -1429,7 +1447,7 @@
       <c r="S7" s="29"/>
       <c r="T7" s="29"/>
       <c r="U7" s="30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V7" s="31"/>
       <c r="W7" s="31"/>
@@ -1595,7 +1613,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>17</v>
@@ -1667,7 +1685,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="10"/>
@@ -1702,10 +1720,10 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="18"/>
@@ -1739,10 +1757,10 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B16" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="18"/>
@@ -1776,10 +1794,10 @@
     </row>
     <row r="17" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B17" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>35</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="18"/>
@@ -1813,10 +1831,10 @@
     </row>
     <row r="18" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B18" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="18"/>
@@ -1850,7 +1868,7 @@
     </row>
     <row r="19" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B19" s="12" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="10"/>
@@ -1883,12 +1901,16 @@
       <c r="AE19" s="18"/>
       <c r="AF19" s="18"/>
     </row>
-    <row r="20" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="10"/>
+        <v>35</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>97</v>
+      </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
@@ -1918,12 +1940,16 @@
       <c r="AE20" s="18"/>
       <c r="AF20" s="18"/>
     </row>
-    <row r="21" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="10"/>
+        <v>37</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>100</v>
+      </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
@@ -1935,11 +1961,11 @@
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
       <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
+      <c r="P21" s="19"/>
       <c r="Q21" s="19"/>
       <c r="R21" s="19"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="19"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
       <c r="U21" s="18"/>
       <c r="V21" s="18"/>
       <c r="W21" s="18"/>
@@ -1955,9 +1981,11 @@
     </row>
     <row r="22" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B22" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>101</v>
+      </c>
       <c r="D22" s="10"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
@@ -1972,14 +2000,14 @@
       <c r="O22" s="18"/>
       <c r="P22" s="18"/>
       <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
       <c r="U22" s="19"/>
       <c r="V22" s="19"/>
       <c r="W22" s="19"/>
       <c r="X22" s="19"/>
-      <c r="Y22" s="19"/>
+      <c r="Y22" s="18"/>
       <c r="Z22" s="18"/>
       <c r="AA22" s="18"/>
       <c r="AB22" s="18"/>
@@ -1990,7 +2018,7 @@
     </row>
     <row r="23" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="10"/>
@@ -2028,7 +2056,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="18"/>
@@ -2049,26 +2077,26 @@
       <c r="T24" s="18"/>
       <c r="U24" s="18"/>
       <c r="V24" s="18"/>
-      <c r="W24" s="18"/>
-      <c r="X24" s="18"/>
-      <c r="Y24" s="18"/>
+      <c r="W24" s="19"/>
+      <c r="X24" s="19"/>
+      <c r="Y24" s="19"/>
       <c r="Z24" s="18"/>
       <c r="AA24" s="18"/>
-      <c r="AB24" s="19"/>
-      <c r="AC24" s="19"/>
-      <c r="AD24" s="19"/>
+      <c r="AB24" s="18"/>
+      <c r="AC24" s="18"/>
+      <c r="AD24" s="18"/>
       <c r="AE24" s="18"/>
       <c r="AF24" s="18"/>
     </row>
     <row r="25" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
@@ -2093,11 +2121,11 @@
       <c r="Y25" s="18"/>
       <c r="Z25" s="18"/>
       <c r="AA25" s="18"/>
-      <c r="AB25" s="18"/>
+      <c r="AB25" s="19"/>
       <c r="AC25" s="18"/>
       <c r="AD25" s="18"/>
       <c r="AE25" s="18"/>
-      <c r="AF25" s="19"/>
+      <c r="AF25" s="18"/>
     </row>
     <row r="26" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B26" s="14" t="s">
@@ -2240,28 +2268,28 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>7</v>
@@ -2269,19 +2297,19 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="34"/>
       <c r="B7" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C7" s="34"/>
     </row>
@@ -2293,60 +2321,60 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" s="24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9" s="34"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="34"/>
       <c r="B10" s="24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C10" s="34"/>
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="35"/>
       <c r="B11" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C11" s="35"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="37"/>
       <c r="B13" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13" s="34"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="37"/>
       <c r="B14" s="21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C14" s="34"/>
     </row>
     <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="37"/>
       <c r="B15" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C15" s="34"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="37"/>
       <c r="B16" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C16" s="34"/>
     </row>
@@ -2357,40 +2385,40 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="42" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="43"/>
       <c r="B19" s="23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" s="40"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="43"/>
       <c r="B20" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" s="40"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="43"/>
       <c r="B21" s="23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C21" s="40"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="43"/>
       <c r="B22" s="23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C22" s="40"/>
     </row>
@@ -2401,86 +2429,86 @@
     </row>
     <row r="24" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
       <c r="B25" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C25" s="34"/>
     </row>
     <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="37"/>
       <c r="B26" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C26" s="34"/>
     </row>
     <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="38"/>
       <c r="B27" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C27" s="35"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="37"/>
       <c r="B29" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C29" s="34"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="37"/>
       <c r="B30" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C30" s="34"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="37"/>
       <c r="B31" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C31" s="34"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="37"/>
       <c r="B32" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C32" s="34"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="37"/>
       <c r="B33" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C33" s="34"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="37"/>
       <c r="B34" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C34" s="34"/>
     </row>
@@ -2491,33 +2519,33 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="37"/>
       <c r="B37" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C37" s="34"/>
     </row>
     <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="37"/>
       <c r="B38" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C38" s="34"/>
     </row>
     <row r="39" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="37"/>
       <c r="B39" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C39" s="34"/>
     </row>
@@ -2528,31 +2556,31 @@
     </row>
     <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C41" s="33"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="37"/>
       <c r="B42" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C42" s="34"/>
     </row>
     <row r="43" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="37"/>
       <c r="B43" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C43" s="34"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="38"/>
       <c r="B44" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C44" s="35"/>
     </row>

</xml_diff>